<commit_message>
lower bound catch at length
This file is rec. selectivity, with lower bounds of total catch. Rec. selectivity is calculated using total numbers at length for each state, rather than assigning biomass shares across states
</commit_message>
<xml_diff>
--- a/rec_selectivity_by_state_cdf_star_raw_18_19_lb.xlsx
+++ b/rec_selectivity_by_state_cdf_star_raw_18_19_lb.xlsx
@@ -136,7 +136,7 @@
         <v>413071</v>
       </c>
       <c r="E2" s="1">
-        <v>1.1609237009213569e-11</v>
+        <v>1.9496260075108074e-12</v>
       </c>
     </row>
     <row r="3">
@@ -153,7 +153,7 @@
         <v>413071</v>
       </c>
       <c r="E3" s="1">
-        <v>9.4581330614684767e-13</v>
+        <v>1.5883750207040109e-13</v>
       </c>
     </row>
     <row r="4">
@@ -170,7 +170,7 @@
         <v>413071</v>
       </c>
       <c r="E4" s="1">
-        <v>4.8175863298638433e-09</v>
+        <v>8.0905326882430018e-10</v>
       </c>
     </row>
     <row r="5">
@@ -187,7 +187,7 @@
         <v>413071</v>
       </c>
       <c r="E5" s="1">
-        <v>5.469468433716429e-09</v>
+        <v>9.1852875305775683e-10</v>
       </c>
     </row>
     <row r="6">
@@ -204,7 +204,7 @@
         <v>413071</v>
       </c>
       <c r="E6" s="1">
-        <v>3.1053858151608438e-08</v>
+        <v>5.2151061247229791e-09</v>
       </c>
     </row>
     <row r="7">
@@ -221,7 +221,7 @@
         <v>413071</v>
       </c>
       <c r="E7" s="1">
-        <v>2.4233260731421069e-08</v>
+        <v>4.0696725989164406e-09</v>
       </c>
     </row>
     <row r="8">
@@ -238,7 +238,7 @@
         <v>413071</v>
       </c>
       <c r="E8" s="1">
-        <v>1.0912947345786961e-07</v>
+        <v>1.8326927531120418e-08</v>
       </c>
     </row>
     <row r="9">
@@ -255,7 +255,7 @@
         <v>413071</v>
       </c>
       <c r="E9" s="1">
-        <v>2.0448227644465078e-07</v>
+        <v>3.4340235544050302e-08</v>
       </c>
     </row>
     <row r="10">
@@ -272,7 +272,7 @@
         <v>413071</v>
       </c>
       <c r="E10" s="1">
-        <v>1.5778584838699317e-07</v>
+        <v>2.6498158334220534e-08</v>
       </c>
     </row>
     <row r="11">
@@ -289,7 +289,7 @@
         <v>413071</v>
       </c>
       <c r="E11" s="1">
-        <v>9.0275435127296078e-08</v>
+        <v>1.5160628308308333e-08</v>
       </c>
     </row>
     <row r="12">
@@ -306,7 +306,7 @@
         <v>413071</v>
       </c>
       <c r="E12" s="1">
-        <v>2.563953671597119e-07</v>
+        <v>4.3058392407147039e-08</v>
       </c>
     </row>
     <row r="13">
@@ -323,7 +323,7 @@
         <v>413071</v>
       </c>
       <c r="E13" s="1">
-        <v>2.9210275442892453e-07</v>
+        <v>4.9054996509312332e-08</v>
       </c>
     </row>
     <row r="14">
@@ -340,7 +340,7 @@
         <v>413071</v>
       </c>
       <c r="E14" s="1">
-        <v>4.1772989334276645e-07</v>
+        <v>7.0152502473774803e-08</v>
       </c>
     </row>
     <row r="15">
@@ -357,7 +357,7 @@
         <v>413071</v>
       </c>
       <c r="E15" s="1">
-        <v>1.1331883342791116e-07</v>
+        <v>1.9030478526360639e-08</v>
       </c>
     </row>
     <row r="16">
@@ -374,7 +374,7 @@
         <v>413071</v>
       </c>
       <c r="E16" s="1">
-        <v>5.9132027274699794e-08</v>
+        <v>9.9304831024937812e-09</v>
       </c>
     </row>
     <row r="17">
@@ -391,7 +391,7 @@
         <v>413071</v>
       </c>
       <c r="E17" s="1">
-        <v>9.0155587884055421e-08</v>
+        <v>1.5140502185317928e-08</v>
       </c>
     </row>
     <row r="18">
@@ -408,7 +408,7 @@
         <v>413071</v>
       </c>
       <c r="E18" s="1">
-        <v>3.7749348535953686e-08</v>
+        <v>6.3395302341007209e-09</v>
       </c>
     </row>
     <row r="19">
@@ -425,7 +425,7 @@
         <v>413071</v>
       </c>
       <c r="E19" s="1">
-        <v>3.0505393766588895e-08</v>
+        <v>5.1229984698863973e-09</v>
       </c>
     </row>
     <row r="20">
@@ -442,7 +442,7 @@
         <v>413071</v>
       </c>
       <c r="E20" s="1">
-        <v>1.9147689656051625e-08</v>
+        <v>3.2156146634321203e-09</v>
       </c>
     </row>
     <row r="21">
@@ -459,7 +459,7 @@
         <v>413071</v>
       </c>
       <c r="E21" s="1">
-        <v>7.1710157811821773e-09</v>
+        <v>1.2042823405167269e-09</v>
       </c>
     </row>
     <row r="22">
@@ -476,7 +476,7 @@
         <v>413071</v>
       </c>
       <c r="E22" s="1">
-        <v>1.701315643920509e-09</v>
+        <v>2.8571464638638133e-10</v>
       </c>
     </row>
     <row r="23">
@@ -493,7 +493,7 @@
         <v>413071</v>
       </c>
       <c r="E23" s="1">
-        <v>8.3771185543923821e-09</v>
+        <v>1.4068322062854577e-09</v>
       </c>
     </row>
     <row r="24">
@@ -510,7 +510,7 @@
         <v>413071</v>
       </c>
       <c r="E24" s="1">
-        <v>1.3217958283462394e-08</v>
+        <v>2.2197905735765744e-09</v>
       </c>
     </row>
     <row r="25">
@@ -527,7 +527,7 @@
         <v>413071</v>
       </c>
       <c r="E25" s="1">
-        <v>9.9037306133809011e-11</v>
+        <v>1.6632075924838396e-11</v>
       </c>
     </row>
     <row r="26">
@@ -544,7 +544,7 @@
         <v>413071</v>
       </c>
       <c r="E26" s="1">
-        <v>7.2502892578540923e-09</v>
+        <v>1.2175952468496121e-09</v>
       </c>
     </row>
     <row r="27">
@@ -561,7 +561,7 @@
         <v>413071</v>
       </c>
       <c r="E27" s="1">
-        <v>3.7844777311946132e-10</v>
+        <v>6.3555563589723363e-11</v>
       </c>
     </row>
     <row r="28">
@@ -578,7 +578,7 @@
         <v>401288</v>
       </c>
       <c r="E28" s="1">
-        <v>5.5119631081623766e-11</v>
+        <v>2.00687274957978e-12</v>
       </c>
     </row>
     <row r="29">
@@ -595,7 +595,7 @@
         <v>401288</v>
       </c>
       <c r="E29" s="1">
-        <v>1.5229533190108668e-08</v>
+        <v>5.544981696026241e-10</v>
       </c>
     </row>
     <row r="30">
@@ -612,7 +612,7 @@
         <v>401288</v>
       </c>
       <c r="E30" s="1">
-        <v>1.2779595159884138e-08</v>
+        <v>4.6529738395584275e-10</v>
       </c>
     </row>
     <row r="31">
@@ -629,7 +629,7 @@
         <v>401288</v>
       </c>
       <c r="E31" s="1">
-        <v>1.692698248234592e-08</v>
+        <v>6.1630128778134008e-10</v>
       </c>
     </row>
     <row r="32">
@@ -646,7 +646,7 @@
         <v>401288</v>
       </c>
       <c r="E32" s="1">
-        <v>8.6497514928396413e-08</v>
+        <v>3.1493225804979375e-09</v>
       </c>
     </row>
     <row r="33">
@@ -663,7 +663,7 @@
         <v>401288</v>
       </c>
       <c r="E33" s="1">
-        <v>1.7999985857386491e-07</v>
+        <v>6.5536869264803954e-09</v>
       </c>
     </row>
     <row r="34">
@@ -680,7 +680,7 @@
         <v>401288</v>
       </c>
       <c r="E34" s="1">
-        <v>4.6607473791482334e-07</v>
+        <v>1.6969501359653805e-08</v>
       </c>
     </row>
     <row r="35">
@@ -697,7 +697,7 @@
         <v>401288</v>
       </c>
       <c r="E35" s="1">
-        <v>5.8750526932271896e-07</v>
+        <v>2.1390714977087555e-08</v>
       </c>
     </row>
     <row r="36">
@@ -714,7 +714,7 @@
         <v>401288</v>
       </c>
       <c r="E36" s="1">
-        <v>6.6370051854391932e-07</v>
+        <v>2.4164938494664057e-08</v>
       </c>
     </row>
     <row r="37">
@@ -731,7 +731,7 @@
         <v>401288</v>
       </c>
       <c r="E37" s="1">
-        <v>3.8391513612623385e-07</v>
+        <v>1.3978119994817462e-08</v>
       </c>
     </row>
     <row r="38">
@@ -748,7 +748,7 @@
         <v>401288</v>
       </c>
       <c r="E38" s="1">
-        <v>3.7467827951331856e-07</v>
+        <v>1.3641811236198009e-08</v>
       </c>
     </row>
     <row r="39">
@@ -765,7 +765,7 @@
         <v>401288</v>
       </c>
       <c r="E39" s="1">
-        <v>1.9302206055726856e-07</v>
+        <v>7.0278174391091852e-09</v>
       </c>
     </row>
     <row r="40">
@@ -782,7 +782,7 @@
         <v>401288</v>
       </c>
       <c r="E40" s="1">
-        <v>2.4946660914793028e-07</v>
+        <v>9.0829299637107397e-09</v>
       </c>
     </row>
     <row r="41">
@@ -799,7 +799,7 @@
         <v>401288</v>
       </c>
       <c r="E41" s="1">
-        <v>1.4480521315363148e-07</v>
+        <v>5.2722706200825087e-09</v>
       </c>
     </row>
     <row r="42">
@@ -816,7 +816,7 @@
         <v>401288</v>
       </c>
       <c r="E42" s="1">
-        <v>6.0669243850952626e-08</v>
+        <v>2.208930593994296e-09</v>
       </c>
     </row>
     <row r="43">
@@ -833,7 +833,7 @@
         <v>401288</v>
       </c>
       <c r="E43" s="1">
-        <v>4.0886909857817955e-08</v>
+        <v>1.4886678556536026e-09</v>
       </c>
     </row>
     <row r="44">
@@ -850,7 +850,7 @@
         <v>401288</v>
       </c>
       <c r="E44" s="1">
-        <v>6.9342675601546944e-08</v>
+        <v>2.5247250956539347e-09</v>
       </c>
     </row>
     <row r="45">
@@ -867,7 +867,7 @@
         <v>401288</v>
       </c>
       <c r="E45" s="1">
-        <v>7.8573908490753297e-10</v>
+        <v>2.8608287613862693e-11</v>
       </c>
     </row>
     <row r="46">
@@ -884,7 +884,7 @@
         <v>401288</v>
       </c>
       <c r="E46" s="1">
-        <v>7.5555357526013722e-09</v>
+        <v>2.7509253208712892e-10</v>
       </c>
     </row>
     <row r="47">
@@ -901,7 +901,7 @@
         <v>401288</v>
       </c>
       <c r="E47" s="1">
-        <v>1.1620807427448199e-08</v>
+        <v>4.231066053073107e-10</v>
       </c>
     </row>
     <row r="48">
@@ -918,7 +918,7 @@
         <v>401288</v>
       </c>
       <c r="E48" s="1">
-        <v>5.6791225944152757e-08</v>
+        <v>2.0677344281239129e-09</v>
       </c>
     </row>
     <row r="49">
@@ -935,7 +935,7 @@
         <v>401288</v>
       </c>
       <c r="E49" s="1">
-        <v>1.6305864991572605e-10</v>
+        <v>5.9368677508830903e-12</v>
       </c>
     </row>
     <row r="50">
@@ -952,7 +952,7 @@
         <v>401288</v>
       </c>
       <c r="E50" s="1">
-        <v>1.6104542699402202e-10</v>
+        <v>5.8635674440865593e-12</v>
       </c>
     </row>
     <row r="51">
@@ -969,7 +969,7 @@
         <v>401288</v>
       </c>
       <c r="E51" s="1">
-        <v>4.7022036264721123e-10</v>
+        <v>1.7120442216689291e-11</v>
       </c>
     </row>
     <row r="52">
@@ -986,7 +986,7 @@
         <v>401288</v>
       </c>
       <c r="E52" s="1">
-        <v>1.1978910086085648e-09</v>
+        <v>4.3614493960841827e-11</v>
       </c>
     </row>
     <row r="53">
@@ -1003,7 +1003,7 @@
         <v>401288</v>
       </c>
       <c r="E53" s="1">
-        <v>1.7968365684239984e-09</v>
+        <v>6.5421744410709692e-11</v>
       </c>
     </row>
     <row r="54">
@@ -1020,7 +1020,7 @@
         <v>104251</v>
       </c>
       <c r="E54" s="1">
-        <v>4.5998975461980507e-11</v>
+        <v>7.7249517546618129e-12</v>
       </c>
     </row>
     <row r="55">
@@ -1037,7 +1037,7 @@
         <v>104251</v>
       </c>
       <c r="E55" s="1">
-        <v>3.7475712637291547e-12</v>
+        <v>6.2935767708438561e-13</v>
       </c>
     </row>
     <row r="56">
@@ -1054,7 +1054,7 @@
         <v>104251</v>
       </c>
       <c r="E56" s="1">
-        <v>3.1134363750323635e-12</v>
+        <v>5.2286262342340906e-13</v>
       </c>
     </row>
     <row r="57">
@@ -1071,7 +1071,7 @@
         <v>104251</v>
       </c>
       <c r="E57" s="1">
-        <v>2.7492307475701638e-12</v>
+        <v>4.616988757456808e-13</v>
       </c>
     </row>
     <row r="58">
@@ -1088,7 +1088,7 @@
         <v>104251</v>
       </c>
       <c r="E58" s="1">
-        <v>4.7712706674474248e-08</v>
+        <v>8.012751351316183e-09</v>
       </c>
     </row>
     <row r="59">
@@ -1105,7 +1105,7 @@
         <v>104251</v>
       </c>
       <c r="E59" s="1">
-        <v>4.9644278021787613e-08</v>
+        <v>8.3371345382943218e-09</v>
       </c>
     </row>
     <row r="60">
@@ -1122,7 +1122,7 @@
         <v>104251</v>
       </c>
       <c r="E60" s="1">
-        <v>1.3413762189884437e-07</v>
+        <v>2.2526734255734482e-08</v>
       </c>
     </row>
     <row r="61">
@@ -1139,7 +1139,7 @@
         <v>104251</v>
       </c>
       <c r="E61" s="1">
-        <v>2.0200242545342917e-07</v>
+        <v>3.3923779341193949e-08</v>
       </c>
     </row>
     <row r="62">
@@ -1156,7 +1156,7 @@
         <v>104251</v>
       </c>
       <c r="E62" s="1">
-        <v>1.0886462575854239e-07</v>
+        <v>1.8282451108575515e-08</v>
       </c>
     </row>
     <row r="63">
@@ -1173,7 +1173,7 @@
         <v>104251</v>
       </c>
       <c r="E63" s="1">
-        <v>6.5037362162456702e-08</v>
+        <v>1.0922210691433065e-08</v>
       </c>
     </row>
     <row r="64">
@@ -1190,7 +1190,7 @@
         <v>104251</v>
       </c>
       <c r="E64" s="1">
-        <v>4.5898187295279058e-07</v>
+        <v>7.7080258620298991e-08</v>
       </c>
     </row>
     <row r="65">
@@ -1207,7 +1207,7 @@
         <v>104251</v>
       </c>
       <c r="E65" s="1">
-        <v>8.4164248903562111e-08</v>
+        <v>1.413433103891748e-08</v>
       </c>
     </row>
     <row r="66">
@@ -1224,7 +1224,7 @@
         <v>104251</v>
       </c>
       <c r="E66" s="1">
-        <v>9.4323766575143964e-08</v>
+        <v>1.584049513780883e-08</v>
       </c>
     </row>
     <row r="67">
@@ -1241,7 +1241,7 @@
         <v>104251</v>
       </c>
       <c r="E67" s="1">
-        <v>5.5026358580789747e-08</v>
+        <v>9.2409875307453149e-09</v>
       </c>
     </row>
     <row r="68">
@@ -1258,7 +1258,7 @@
         <v>104251</v>
       </c>
       <c r="E68" s="1">
-        <v>1.2426011153365835e-07</v>
+        <v>2.0867929606538382e-08</v>
       </c>
     </row>
     <row r="69">
@@ -1275,7 +1275,7 @@
         <v>104251</v>
       </c>
       <c r="E69" s="1">
-        <v>8.2462811690220406e-08</v>
+        <v>1.3848596935872592e-08</v>
       </c>
     </row>
     <row r="70">
@@ -1292,7 +1292,7 @@
         <v>104251</v>
       </c>
       <c r="E70" s="1">
-        <v>5.0166573117849111e-08</v>
+        <v>8.4248474863102274e-09</v>
       </c>
     </row>
     <row r="71">
@@ -1309,7 +1309,7 @@
         <v>104251</v>
       </c>
       <c r="E71" s="1">
-        <v>5.41029407941096e-08</v>
+        <v>9.085911578665673e-09</v>
       </c>
     </row>
     <row r="72">
@@ -1326,7 +1326,7 @@
         <v>104251</v>
       </c>
       <c r="E72" s="1">
-        <v>1.0520493809451636e-08</v>
+        <v>1.7667851626157471e-09</v>
       </c>
     </row>
     <row r="73">
@@ -1343,7 +1343,7 @@
         <v>104251</v>
       </c>
       <c r="E73" s="1">
-        <v>6.3078008094574756e-11</v>
+        <v>1.0593161764438364e-11</v>
       </c>
     </row>
     <row r="74">
@@ -1360,7 +1360,7 @@
         <v>104251</v>
       </c>
       <c r="E74" s="1">
-        <v>6.2490672358972432e-11</v>
+        <v>1.049452625495606e-11</v>
       </c>
     </row>
     <row r="75">
@@ -1377,7 +1377,7 @@
         <v>104251</v>
       </c>
       <c r="E75" s="1">
-        <v>5.3731019633573851e-09</v>
+        <v>9.0234519856124962e-10</v>
       </c>
     </row>
     <row r="76">
@@ -1394,7 +1394,7 @@
         <v>104251</v>
       </c>
       <c r="E76" s="1">
-        <v>1.3439720170094205e-10</v>
+        <v>2.2570327551374447e-11</v>
       </c>
     </row>
     <row r="77">
@@ -1411,7 +1411,7 @@
         <v>104251</v>
       </c>
       <c r="E77" s="1">
-        <v>3.9241293547931377e-10</v>
+        <v>6.5900833401411063e-11</v>
       </c>
     </row>
     <row r="78">
@@ -1428,7 +1428,7 @@
         <v>104251</v>
       </c>
       <c r="E78" s="1">
-        <v>9.9967567557257553e-10</v>
+        <v>1.6788301304693221e-10</v>
       </c>
     </row>
     <row r="79">
@@ -1445,7 +1445,7 @@
         <v>104251</v>
       </c>
       <c r="E79" s="1">
-        <v>1.4995137354034682e-09</v>
+        <v>2.5182453344818612e-10</v>
       </c>
     </row>
     <row r="80">
@@ -1462,7 +1462,7 @@
         <v>544681</v>
       </c>
       <c r="E80" s="1">
-        <v>8.8625000671527232e-07</v>
+        <v>3.2267831073795605e-08</v>
       </c>
     </row>
     <row r="81">
@@ -1479,7 +1479,7 @@
         <v>544681</v>
       </c>
       <c r="E81" s="1">
-        <v>1.241248952510432e-07</v>
+        <v>4.519312923889629e-09</v>
       </c>
     </row>
     <row r="82">
@@ -1496,7 +1496,7 @@
         <v>544681</v>
       </c>
       <c r="E82" s="1">
-        <v>1.1417553480441711e-07</v>
+        <v>4.1570626940767852e-09</v>
       </c>
     </row>
     <row r="83">
@@ -1513,7 +1513,7 @@
         <v>544681</v>
       </c>
       <c r="E83" s="1">
-        <v>1.3082633643080044e-07</v>
+        <v>4.7633084143683391e-09</v>
       </c>
     </row>
     <row r="84">
@@ -1530,7 +1530,7 @@
         <v>544681</v>
       </c>
       <c r="E84" s="1">
-        <v>5.9813010011566803e-07</v>
+        <v>2.1777559311431105e-08</v>
       </c>
     </row>
     <row r="85">
@@ -1547,7 +1547,7 @@
         <v>544681</v>
       </c>
       <c r="E85" s="1">
-        <v>1.0811530728460639e-06</v>
+        <v>3.9364135062669448e-08</v>
       </c>
     </row>
     <row r="86">
@@ -1564,7 +1564,7 @@
         <v>544681</v>
       </c>
       <c r="E86" s="1">
-        <v>9.2109900151626789e-07</v>
+        <v>3.3536661447897131e-08</v>
       </c>
     </row>
     <row r="87">
@@ -1581,7 +1581,7 @@
         <v>544681</v>
       </c>
       <c r="E87" s="1">
-        <v>3.7012949860582012e-07</v>
+        <v>1.3476192606276527e-08</v>
       </c>
     </row>
     <row r="88">
@@ -1598,7 +1598,7 @@
         <v>544681</v>
       </c>
       <c r="E88" s="1">
-        <v>2.2309389180463768e-07</v>
+        <v>8.1227140569239964e-09</v>
       </c>
     </row>
     <row r="89">
@@ -1615,7 +1615,7 @@
         <v>544681</v>
       </c>
       <c r="E89" s="1">
-        <v>1.3575638035945303e-07</v>
+        <v>4.9428083848113147e-09</v>
       </c>
     </row>
     <row r="90">
@@ -1632,7 +1632,7 @@
         <v>544681</v>
       </c>
       <c r="E90" s="1">
-        <v>1.4344581700242998e-07</v>
+        <v>5.2227759894662995e-09</v>
       </c>
     </row>
     <row r="91">
@@ -1649,7 +1649,7 @@
         <v>544681</v>
       </c>
       <c r="E91" s="1">
-        <v>1.5682861942423187e-07</v>
+        <v>5.7100359995843064e-09</v>
       </c>
     </row>
     <row r="92">
@@ -1666,7 +1666,7 @@
         <v>544681</v>
       </c>
       <c r="E92" s="1">
-        <v>1.4170856843520596e-07</v>
+        <v>5.1595239192181452e-09</v>
       </c>
     </row>
     <row r="93">
@@ -1683,7 +1683,7 @@
         <v>544681</v>
       </c>
       <c r="E93" s="1">
-        <v>1.4894729361003556e-07</v>
+        <v>5.4230815393907505e-09</v>
       </c>
     </row>
     <row r="94">
@@ -1700,7 +1700,7 @@
         <v>544681</v>
       </c>
       <c r="E94" s="1">
-        <v>9.3795748057345918e-08</v>
+        <v>3.4150469119254012e-09</v>
       </c>
     </row>
     <row r="95">
@@ -1717,7 +1717,7 @@
         <v>544681</v>
       </c>
       <c r="E95" s="1">
-        <v>3.7868275626351533e-08</v>
+        <v>1.3787612163085328e-09</v>
       </c>
     </row>
     <row r="96">
@@ -1734,7 +1734,7 @@
         <v>544681</v>
       </c>
       <c r="E96" s="1">
-        <v>1.9370913761918018e-08</v>
+        <v>7.0528333173669466e-10</v>
       </c>
     </row>
     <row r="97">
@@ -1751,7 +1751,7 @@
         <v>544681</v>
       </c>
       <c r="E97" s="1">
-        <v>4.9430615156609292e-09</v>
+        <v>1.7997391077440028e-10</v>
       </c>
     </row>
     <row r="98">
@@ -1768,7 +1768,7 @@
         <v>544681</v>
       </c>
       <c r="E98" s="1">
-        <v>2.5409620588168202e-11</v>
+        <v>9.2514906326057744e-13</v>
       </c>
     </row>
     <row r="99">
@@ -1785,7 +1785,7 @@
         <v>544681</v>
       </c>
       <c r="E99" s="1">
-        <v>6.6314724544991321e-11</v>
+        <v>2.4144792068470089e-12</v>
       </c>
     </row>
     <row r="100">
@@ -1802,7 +1802,7 @@
         <v>544681</v>
       </c>
       <c r="E100" s="1">
-        <v>2.3818614636184066e-08</v>
+        <v>8.6722146130924216e-10</v>
       </c>
     </row>
     <row r="101">
@@ -1819,7 +1819,7 @@
         <v>544681</v>
       </c>
       <c r="E101" s="1">
-        <v>1.201317517685041e-10</v>
+        <v>4.3739248334340175e-12</v>
       </c>
     </row>
     <row r="102">
@@ -1836,7 +1836,7 @@
         <v>544681</v>
       </c>
       <c r="E102" s="1">
-        <v>1.1864852156318051e-10</v>
+        <v>4.3199215905842525e-12</v>
       </c>
     </row>
     <row r="103">
@@ -1853,7 +1853,7 @@
         <v>544681</v>
       </c>
       <c r="E103" s="1">
-        <v>3.4642991253441835e-10</v>
+        <v>1.2613305365449801e-11</v>
       </c>
     </row>
     <row r="104">
@@ -1870,7 +1870,7 @@
         <v>544681</v>
       </c>
       <c r="E104" s="1">
-        <v>8.8253360175372109e-10</v>
+        <v>3.2132518867911131e-11</v>
       </c>
     </row>
     <row r="105">
@@ -1887,7 +1887,7 @@
         <v>544681</v>
       </c>
       <c r="E105" s="1">
-        <v>1.3238005136528841e-09</v>
+        <v>4.8198781771313648e-11</v>
       </c>
     </row>
     <row r="106">
@@ -1904,7 +1904,7 @@
         <v>26646</v>
       </c>
       <c r="E106" s="1">
-        <v>1.1147278655698756e-07</v>
+        <v>4.0586574101553197e-09</v>
       </c>
     </row>
     <row r="107">
@@ -1921,7 +1921,7 @@
         <v>26646</v>
       </c>
       <c r="E107" s="1">
-        <v>7.6531261328227629e-09</v>
+        <v>2.7864571761071488e-10</v>
       </c>
     </row>
     <row r="108">
@@ -1938,7 +1938,7 @@
         <v>26646</v>
       </c>
       <c r="E108" s="1">
-        <v>7.0396826146179592e-09</v>
+        <v>2.5631061162378899e-10</v>
       </c>
     </row>
     <row r="109">
@@ -1955,7 +1955,7 @@
         <v>26646</v>
       </c>
       <c r="E109" s="1">
-        <v>8.0663156154514581e-09</v>
+        <v>2.9368971143917122e-10</v>
       </c>
     </row>
     <row r="110">
@@ -1972,7 +1972,7 @@
         <v>26646</v>
       </c>
       <c r="E110" s="1">
-        <v>3.687870631097212e-08</v>
+        <v>1.3427315925795824e-09</v>
       </c>
     </row>
     <row r="111">
@@ -1989,7 +1989,7 @@
         <v>26646</v>
       </c>
       <c r="E111" s="1">
-        <v>6.6660291508924274e-08</v>
+        <v>2.4270609966237089e-09</v>
       </c>
     </row>
     <row r="112">
@@ -2006,7 +2006,7 @@
         <v>26646</v>
       </c>
       <c r="E112" s="1">
-        <v>5.6791890301610692e-08</v>
+        <v>2.0677586309858498e-09</v>
       </c>
     </row>
     <row r="113">
@@ -2023,7 +2023,7 @@
         <v>26646</v>
       </c>
       <c r="E113" s="1">
-        <v>2.2820950462687506e-08</v>
+        <v>8.3089707336725382e-10</v>
       </c>
     </row>
     <row r="114">
@@ -2040,7 +2040,7 @@
         <v>26646</v>
       </c>
       <c r="E114" s="1">
-        <v>7.0059407164535514e-09</v>
+        <v>2.5508209433589002e-10</v>
       </c>
     </row>
     <row r="115">
@@ -2057,7 +2057,7 @@
         <v>26646</v>
       </c>
       <c r="E115" s="1">
-        <v>5.1409517709544161e-07</v>
+        <v>1.8717896566045056e-08</v>
       </c>
     </row>
     <row r="116">
@@ -2074,7 +2074,7 @@
         <v>26646</v>
       </c>
       <c r="E116" s="1">
-        <v>5.4317672493198188e-07</v>
+        <v>1.977673846909056e-08</v>
       </c>
     </row>
     <row r="117">
@@ -2091,7 +2091,7 @@
         <v>26646</v>
       </c>
       <c r="E117" s="1">
-        <v>6.0002616919518914e-07</v>
+        <v>2.1846593867280717e-08</v>
       </c>
     </row>
     <row r="118">
@@ -2108,7 +2108,7 @@
         <v>26646</v>
       </c>
       <c r="E118" s="1">
-        <v>5.4217690603763913e-07</v>
+        <v>1.9740335588380731e-08</v>
       </c>
     </row>
     <row r="119">
@@ -2125,7 +2125,7 @@
         <v>26646</v>
       </c>
       <c r="E119" s="1">
-        <v>5.6987227026183973e-07</v>
+        <v>2.0748707640905195e-08</v>
       </c>
     </row>
     <row r="120">
@@ -2142,7 +2142,7 @@
         <v>26646</v>
       </c>
       <c r="E120" s="1">
-        <v>3.5886247928829107e-07</v>
+        <v>1.3065967863212791e-08</v>
       </c>
     </row>
     <row r="121">
@@ -2159,7 +2159,7 @@
         <v>26646</v>
       </c>
       <c r="E121" s="1">
-        <v>1.4488399813217256e-07</v>
+        <v>5.2751394363781401e-09</v>
       </c>
     </row>
     <row r="122">
@@ -2176,7 +2176,7 @@
         <v>26646</v>
       </c>
       <c r="E122" s="1">
-        <v>7.4113103210038389e-08</v>
+        <v>2.6984134926522074e-09</v>
       </c>
     </row>
     <row r="123">
@@ -2193,7 +2193,7 @@
         <v>26646</v>
       </c>
       <c r="E123" s="1">
-        <v>1.891215184457451e-08</v>
+        <v>6.8858008184236041e-10</v>
       </c>
     </row>
     <row r="124">
@@ -2210,7 +2210,7 @@
         <v>26646</v>
       </c>
       <c r="E124" s="1">
-        <v>5.1940768353020417e-10</v>
+        <v>1.8911322161030419e-11</v>
       </c>
     </row>
     <row r="125">
@@ -2227,7 +2227,7 @@
         <v>26646</v>
       </c>
       <c r="E125" s="1">
-        <v>2.5372007272927988e-10</v>
+        <v>9.2377962918055445e-12</v>
       </c>
     </row>
     <row r="126">
@@ -2244,7 +2244,7 @@
         <v>26646</v>
       </c>
       <c r="E126" s="1">
-        <v>9.1130011981022108e-08</v>
+        <v>3.3179889946666208e-09</v>
       </c>
     </row>
     <row r="127">
@@ -2261,7 +2261,7 @@
         <v>26646</v>
       </c>
       <c r="E127" s="1">
-        <v>2.4556585653812135e-09</v>
+        <v>8.9409056547307131e-11</v>
       </c>
     </row>
     <row r="128">
@@ -2278,7 +2278,7 @@
         <v>26646</v>
       </c>
       <c r="E128" s="1">
-        <v>2.4253394848017251e-09</v>
+        <v>8.8305154855028434e-11</v>
       </c>
     </row>
     <row r="129">
@@ -2295,7 +2295,7 @@
         <v>26646</v>
       </c>
       <c r="E129" s="1">
-        <v>7.0815056041340085e-09</v>
+        <v>2.5783336576878924e-10</v>
       </c>
     </row>
     <row r="130">
@@ -2312,7 +2312,7 @@
         <v>26646</v>
       </c>
       <c r="E130" s="1">
-        <v>1.8040203997315984e-08</v>
+        <v>6.5683303240859914e-10</v>
       </c>
     </row>
     <row r="131">
@@ -2329,7 +2329,7 @@
         <v>26646</v>
       </c>
       <c r="E131" s="1">
-        <v>2.7060307772330816e-08</v>
+        <v>9.8524954861289871e-10</v>
       </c>
     </row>
     <row r="132">
@@ -2346,7 +2346,7 @@
         <v>4579196</v>
       </c>
       <c r="E132" s="1">
-        <v>1.0986700438309072e-08</v>
+        <v>2.0063100070188966e-09</v>
       </c>
     </row>
     <row r="133">
@@ -2363,7 +2363,7 @@
         <v>4579196</v>
       </c>
       <c r="E133" s="1">
-        <v>6.0536553547763106e-10</v>
+        <v>1.1054736986926272e-10</v>
       </c>
     </row>
     <row r="134">
@@ -2380,7 +2380,7 @@
         <v>4579196</v>
       </c>
       <c r="E134" s="1">
-        <v>1.0058605059981574e-09</v>
+        <v>1.8368280507718993e-10</v>
       </c>
     </row>
     <row r="135">
@@ -2397,7 +2397,7 @@
         <v>4579196</v>
       </c>
       <c r="E135" s="1">
-        <v>3.3307359093015521e-09</v>
+        <v>6.0823435177326246e-10</v>
       </c>
     </row>
     <row r="136">
@@ -2414,7 +2414,7 @@
         <v>4579196</v>
       </c>
       <c r="E136" s="1">
-        <v>4.8506279881621595e-08</v>
+        <v>8.8578575585529506e-09</v>
       </c>
     </row>
     <row r="137">
@@ -2431,7 +2431,7 @@
         <v>4579196</v>
       </c>
       <c r="E137" s="1">
-        <v>1.1583061620967783e-07</v>
+        <v>2.1152128937274028e-08</v>
       </c>
     </row>
     <row r="138">
@@ -2448,7 +2448,7 @@
         <v>4579196</v>
       </c>
       <c r="E138" s="1">
-        <v>2.9347168606363994e-07</v>
+        <v>5.3591627136029274e-08</v>
       </c>
     </row>
     <row r="139">
@@ -2465,7 +2465,7 @@
         <v>4579196</v>
       </c>
       <c r="E139" s="1">
-        <v>2.2467752103239036e-07</v>
+        <v>4.1028947350696399e-08</v>
       </c>
     </row>
     <row r="140">
@@ -2482,7 +2482,7 @@
         <v>4579196</v>
       </c>
       <c r="E140" s="1">
-        <v>2.1160833796329825e-07</v>
+        <v>3.8642347988115944e-08</v>
       </c>
     </row>
     <row r="141">
@@ -2499,7 +2499,7 @@
         <v>4579196</v>
       </c>
       <c r="E141" s="1">
-        <v>1.1999544824448094e-07</v>
+        <v>2.1912681447133764e-08</v>
       </c>
     </row>
     <row r="142">
@@ -2516,7 +2516,7 @@
         <v>4579196</v>
       </c>
       <c r="E142" s="1">
-        <v>2.4302863721459289e-07</v>
+        <v>4.4380094266216474e-08</v>
       </c>
     </row>
     <row r="143">
@@ -2533,7 +2533,7 @@
         <v>4579196</v>
       </c>
       <c r="E143" s="1">
-        <v>2.2622354833856662e-07</v>
+        <v>4.1311270848609638e-08</v>
       </c>
     </row>
     <row r="144">
@@ -2550,7 +2550,7 @@
         <v>4579196</v>
       </c>
       <c r="E144" s="1">
-        <v>1.2257983428298758e-07</v>
+        <v>2.2384622155868783e-08</v>
       </c>
     </row>
     <row r="145">
@@ -2567,7 +2567,7 @@
         <v>4579196</v>
       </c>
       <c r="E145" s="1">
-        <v>5.1081830321209054e-08</v>
+        <v>9.3281853352777944e-09</v>
       </c>
     </row>
     <row r="146">
@@ -2584,7 +2584,7 @@
         <v>4579196</v>
       </c>
       <c r="E146" s="1">
-        <v>3.6613258203033183e-08</v>
+        <v>6.6860419423164785e-09</v>
       </c>
     </row>
     <row r="147">
@@ -2601,7 +2601,7 @@
         <v>4579196</v>
       </c>
       <c r="E147" s="1">
-        <v>4.1328458877387675e-08</v>
+        <v>7.5470971694358013e-09</v>
       </c>
     </row>
     <row r="148">
@@ -2618,7 +2618,7 @@
         <v>4579196</v>
       </c>
       <c r="E148" s="1">
-        <v>1.9900346259760227e-08</v>
+        <v>3.6340539466550581e-09</v>
       </c>
     </row>
     <row r="149">
@@ -2635,7 +2635,7 @@
         <v>4579196</v>
       </c>
       <c r="E149" s="1">
-        <v>9.6428109941371076e-09</v>
+        <v>1.760898871161487e-09</v>
       </c>
     </row>
     <row r="150">
@@ -2652,7 +2652,7 @@
         <v>4579196</v>
       </c>
       <c r="E150" s="1">
-        <v>1.6993798368503121e-08</v>
+        <v>3.1032816316667322e-09</v>
       </c>
     </row>
     <row r="151">
@@ -2669,7 +2669,7 @@
         <v>4579196</v>
       </c>
       <c r="E151" s="1">
-        <v>3.2319761089638632e-08</v>
+        <v>5.9019953368988354e-09</v>
       </c>
     </row>
     <row r="152">
@@ -2686,7 +2686,7 @@
         <v>4579196</v>
       </c>
       <c r="E152" s="1">
-        <v>6.5276131167024687e-09</v>
+        <v>1.1920243681018405e-09</v>
       </c>
     </row>
     <row r="153">
@@ -2703,7 +2703,7 @@
         <v>4579196</v>
       </c>
       <c r="E153" s="1">
-        <v>7.6030420848027802e-10</v>
+        <v>1.3884113303497259e-10</v>
       </c>
     </row>
     <row r="154">
@@ -2720,7 +2720,7 @@
         <v>4579196</v>
       </c>
       <c r="E154" s="1">
-        <v>2.8138316329751056e-12</v>
+        <v>5.1384113977648305e-13</v>
       </c>
     </row>
     <row r="155">
@@ -2737,7 +2737,7 @@
         <v>4579196</v>
       </c>
       <c r="E155" s="1">
-        <v>1.0961834995271147e-08</v>
+        <v>2.0017691948481797e-09</v>
       </c>
     </row>
     <row r="156">
@@ -2754,7 +2754,7 @@
         <v>4579196</v>
       </c>
       <c r="E156" s="1">
-        <v>2.9530184519899194e-08</v>
+        <v>5.3925837129042975e-09</v>
       </c>
     </row>
     <row r="157">
@@ -2771,7 +2771,7 @@
         <v>4579196</v>
       </c>
       <c r="E157" s="1">
-        <v>4.429528033256247e-08</v>
+        <v>8.088876235490261e-09</v>
       </c>
     </row>
     <row r="158">
@@ -2788,7 +2788,7 @@
         <v>3474730</v>
       </c>
       <c r="E158" s="1">
-        <v>5.0761301828572414e-09</v>
+        <v>8.5247248149400434e-10</v>
       </c>
     </row>
     <row r="159">
@@ -2805,7 +2805,7 @@
         <v>3474730</v>
       </c>
       <c r="E159" s="1">
-        <v>1.9046280108625524e-09</v>
+        <v>3.1985841753012778e-10</v>
       </c>
     </row>
     <row r="160">
@@ -2822,7 +2822,7 @@
         <v>3474730</v>
       </c>
       <c r="E160" s="1">
-        <v>2.2856045944763537e-09</v>
+        <v>3.8383865530455807e-10</v>
       </c>
     </row>
     <row r="161">
@@ -2839,7 +2839,7 @@
         <v>3474730</v>
       </c>
       <c r="E161" s="1">
-        <v>3.2602300858997069e-09</v>
+        <v>5.4751481126658064e-10</v>
       </c>
     </row>
     <row r="162">
@@ -2856,7 +2856,7 @@
         <v>3474730</v>
       </c>
       <c r="E162" s="1">
-        <v>2.8162430609768307e-08</v>
+        <v>4.7295274363534645e-09</v>
       </c>
     </row>
     <row r="163">
@@ -2873,7 +2873,7 @@
         <v>3474730</v>
       </c>
       <c r="E163" s="1">
-        <v>1.0198683497719685e-07</v>
+        <v>1.712741060089229e-08</v>
       </c>
     </row>
     <row r="164">
@@ -2890,7 +2890,7 @@
         <v>3474730</v>
       </c>
       <c r="E164" s="1">
-        <v>2.3496980361414899e-07</v>
+        <v>3.9460235967681001e-08</v>
       </c>
     </row>
     <row r="165">
@@ -2907,7 +2907,7 @@
         <v>3474730</v>
       </c>
       <c r="E165" s="1">
-        <v>2.4291981048918387e-07</v>
+        <v>4.0795338662746872e-08</v>
       </c>
     </row>
     <row r="166">
@@ -2924,7 +2924,7 @@
         <v>3474730</v>
       </c>
       <c r="E166" s="1">
-        <v>2.1788672199818393e-07</v>
+        <v>3.6591345065062342e-08</v>
       </c>
     </row>
     <row r="167">
@@ -2941,7 +2941,7 @@
         <v>3474730</v>
       </c>
       <c r="E167" s="1">
-        <v>1.3384186559051159e-07</v>
+        <v>2.2477063765791172e-08</v>
       </c>
     </row>
     <row r="168">
@@ -2958,7 +2958,7 @@
         <v>3474730</v>
       </c>
       <c r="E168" s="1">
-        <v>2.2090603124524932e-07</v>
+        <v>3.7098402572155464e-08</v>
       </c>
     </row>
     <row r="169">
@@ -2975,7 +2975,7 @@
         <v>3474730</v>
       </c>
       <c r="E169" s="1">
-        <v>1.5365486660812167e-07</v>
+        <v>2.5804411052376963e-08</v>
       </c>
     </row>
     <row r="170">
@@ -2992,7 +2992,7 @@
         <v>3474730</v>
       </c>
       <c r="E170" s="1">
-        <v>1.4759510236217466e-07</v>
+        <v>2.4786748653582436e-08</v>
       </c>
     </row>
     <row r="171">
@@ -3009,7 +3009,7 @@
         <v>3474730</v>
       </c>
       <c r="E171" s="1">
-        <v>5.4210101296803259e-08</v>
+        <v>9.1039069616272172e-09</v>
       </c>
     </row>
     <row r="172">
@@ -3026,7 +3026,7 @@
         <v>3474730</v>
       </c>
       <c r="E172" s="1">
-        <v>3.8500502341776155e-08</v>
+        <v>6.4656768827831002e-09</v>
       </c>
     </row>
     <row r="173">
@@ -3043,7 +3043,7 @@
         <v>3474730</v>
       </c>
       <c r="E173" s="1">
-        <v>7.4874563438243058e-08</v>
+        <v>1.2574244756535791e-08</v>
       </c>
     </row>
     <row r="174">
@@ -3060,7 +3060,7 @@
         <v>3474730</v>
       </c>
       <c r="E174" s="1">
-        <v>4.0353448582663987e-08</v>
+        <v>6.7768559652847671e-09</v>
       </c>
     </row>
     <row r="175">
@@ -3077,7 +3077,7 @@
         <v>3474730</v>
       </c>
       <c r="E175" s="1">
-        <v>4.094153993605687e-08</v>
+        <v>6.8756187410201619e-09</v>
       </c>
     </row>
     <row r="176">
@@ -3094,7 +3094,7 @@
         <v>3474730</v>
       </c>
       <c r="E176" s="1">
-        <v>2.2426959844779049e-08</v>
+        <v>3.7663272500765288e-09</v>
       </c>
     </row>
     <row r="177">
@@ -3111,7 +3111,7 @@
         <v>3474730</v>
       </c>
       <c r="E177" s="1">
-        <v>4.6240042905765222e-08</v>
+        <v>7.7654362939938437e-09</v>
       </c>
     </row>
     <row r="178">
@@ -3128,7 +3128,7 @@
         <v>3474730</v>
       </c>
       <c r="E178" s="1">
-        <v>3.193674302792715e-08</v>
+        <v>5.3633759655724589e-09</v>
       </c>
     </row>
     <row r="179">
@@ -3145,7 +3145,7 @@
         <v>3474730</v>
       </c>
       <c r="E179" s="1">
-        <v>3.4998635101146647e-08</v>
+        <v>5.8775824207657479e-09</v>
       </c>
     </row>
     <row r="180">
@@ -3162,7 +3162,7 @@
         <v>3474730</v>
       </c>
       <c r="E180" s="1">
-        <v>1.7847781919044792e-08</v>
+        <v>2.9973112880554709e-09</v>
       </c>
     </row>
     <row r="181">
@@ -3179,7 +3179,7 @@
         <v>3474730</v>
       </c>
       <c r="E181" s="1">
-        <v>1.7442088662278366e-08</v>
+        <v>2.9291804537479038e-09</v>
       </c>
     </row>
     <row r="182">
@@ -3196,7 +3196,7 @@
         <v>3474730</v>
       </c>
       <c r="E182" s="1">
-        <v>9.5446807790722232e-08</v>
+        <v>1.6029096272518473e-08</v>
       </c>
     </row>
     <row r="183">
@@ -3213,7 +3213,7 @@
         <v>3474730</v>
       </c>
       <c r="E183" s="1">
-        <v>5.2616890400258853e-08</v>
+        <v>8.836347653584653e-09</v>
       </c>
     </row>
     <row r="184">
@@ -3230,7 +3230,7 @@
         <v>472523</v>
       </c>
       <c r="E184" s="1">
-        <v>1.0148583362568075e-11</v>
+        <v>1.704327434390307e-12</v>
       </c>
     </row>
     <row r="185">
@@ -3247,7 +3247,7 @@
         <v>472523</v>
       </c>
       <c r="E185" s="1">
-        <v>8.2681279357788018e-13</v>
+        <v>1.3885285065837194e-13</v>
       </c>
     </row>
     <row r="186">
@@ -3264,7 +3264,7 @@
         <v>472523</v>
       </c>
       <c r="E186" s="1">
-        <v>1.7253517503590388e-09</v>
+        <v>2.8975122301488909e-10</v>
       </c>
     </row>
     <row r="187">
@@ -3281,7 +3281,7 @@
         <v>472523</v>
       </c>
       <c r="E187" s="1">
-        <v>4.5705670359552641e-09</v>
+        <v>7.6756945244227381e-10</v>
       </c>
     </row>
     <row r="188">
@@ -3298,7 +3298,7 @@
         <v>472523</v>
       </c>
       <c r="E188" s="1">
-        <v>1.0380073689475466e-08</v>
+        <v>1.743203359438894e-09</v>
       </c>
     </row>
     <row r="189">
@@ -3315,7 +3315,7 @@
         <v>472523</v>
       </c>
       <c r="E189" s="1">
-        <v>3.7801029861839197e-08</v>
+        <v>6.3482095136180305e-09</v>
       </c>
     </row>
     <row r="190">
@@ -3332,7 +3332,7 @@
         <v>472523</v>
       </c>
       <c r="E190" s="1">
-        <v>1.5112375706394232e-07</v>
+        <v>2.5379343071563198e-08</v>
       </c>
     </row>
     <row r="191">
@@ -3349,7 +3349,7 @@
         <v>472523</v>
       </c>
       <c r="E191" s="1">
-        <v>1.5051391244469414e-07</v>
+        <v>2.5276925441630738e-08</v>
       </c>
     </row>
     <row r="192">
@@ -3366,7 +3366,7 @@
         <v>472523</v>
       </c>
       <c r="E192" s="1">
-        <v>1.2037165220135648e-07</v>
+        <v>2.021491063430858e-08</v>
       </c>
     </row>
     <row r="193">
@@ -3383,7 +3383,7 @@
         <v>472523</v>
       </c>
       <c r="E193" s="1">
-        <v>1.1202507721463917e-07</v>
+        <v>1.8813208768619916e-08</v>
       </c>
     </row>
     <row r="194">
@@ -3400,7 +3400,7 @@
         <v>472523</v>
       </c>
       <c r="E194" s="1">
-        <v>2.3890839884188608e-07</v>
+        <v>4.0121673094972721e-08</v>
       </c>
     </row>
     <row r="195">
@@ -3417,7 +3417,7 @@
         <v>472523</v>
       </c>
       <c r="E195" s="1">
-        <v>2.7406861136114458e-07</v>
+        <v>4.6026389810549517e-08</v>
       </c>
     </row>
     <row r="196">
@@ -3434,7 +3434,7 @@
         <v>472523</v>
       </c>
       <c r="E196" s="1">
-        <v>2.0289250812766113e-07</v>
+        <v>3.4073256216515801e-08</v>
       </c>
     </row>
     <row r="197">
@@ -3451,7 +3451,7 @@
         <v>472523</v>
       </c>
       <c r="E197" s="1">
-        <v>1.1452232939745954e-07</v>
+        <v>1.923259063119076e-08</v>
       </c>
     </row>
     <row r="198">
@@ -3468,7 +3468,7 @@
         <v>472523</v>
       </c>
       <c r="E198" s="1">
-        <v>1.6287613391341438e-07</v>
+        <v>2.7353006970542992e-08</v>
       </c>
     </row>
     <row r="199">
@@ -3485,7 +3485,7 @@
         <v>472523</v>
       </c>
       <c r="E199" s="1">
-        <v>2.6480549308871559e-07</v>
+        <v>4.4470763072013142e-08</v>
       </c>
     </row>
     <row r="200">
@@ -3502,7 +3502,7 @@
         <v>472523</v>
       </c>
       <c r="E200" s="1">
-        <v>5.598488783675748e-08</v>
+        <v>9.4019609875317656e-09</v>
       </c>
     </row>
     <row r="201">
@@ -3519,7 +3519,7 @@
         <v>472523</v>
       </c>
       <c r="E201" s="1">
-        <v>5.8912032585567431e-08</v>
+        <v>9.8935384329479348e-09</v>
       </c>
     </row>
     <row r="202">
@@ -3536,7 +3536,7 @@
         <v>472523</v>
       </c>
       <c r="E202" s="1">
-        <v>7.7546516763504769e-08</v>
+        <v>1.3022966705023009e-08</v>
       </c>
     </row>
     <row r="203">
@@ -3553,7 +3553,7 @@
         <v>472523</v>
       </c>
       <c r="E203" s="1">
-        <v>2.9478352203682334e-08</v>
+        <v>4.950519993940361e-09</v>
       </c>
     </row>
     <row r="204">
@@ -3570,7 +3570,7 @@
         <v>472523</v>
       </c>
       <c r="E204" s="1">
-        <v>3.9432599407973612e-08</v>
+        <v>6.6222112238278896e-09</v>
       </c>
     </row>
     <row r="205">
@@ -3587,7 +3587,7 @@
         <v>472523</v>
       </c>
       <c r="E205" s="1">
-        <v>2.3108397328996944e-07</v>
+        <v>3.880765930830421e-08</v>
       </c>
     </row>
     <row r="206">
@@ -3604,7 +3604,7 @@
         <v>472523</v>
       </c>
       <c r="E206" s="1">
-        <v>1.1781792430554106e-08</v>
+        <v>1.9786043914393758e-09</v>
       </c>
     </row>
     <row r="207">
@@ -3621,7 +3621,7 @@
         <v>472523</v>
       </c>
       <c r="E207" s="1">
-        <v>2.4735280135246285e-07</v>
+        <v>4.1539806261425838e-08</v>
       </c>
     </row>
     <row r="208">
@@ -3638,7 +3638,7 @@
         <v>472523</v>
       </c>
       <c r="E208" s="1">
-        <v>2.5875026565813641e-09</v>
+        <v>4.3453865505860279e-10</v>
       </c>
     </row>
     <row r="209">
@@ -3655,7 +3655,7 @@
         <v>472523</v>
       </c>
       <c r="E209" s="1">
-        <v>3.3083213946127898e-10</v>
+        <v>5.5559116335368586e-11</v>
       </c>
     </row>
     <row r="210">
@@ -3672,7 +3672,7 @@
         <v>785624</v>
       </c>
       <c r="E210" s="1">
-        <v>1.3725472172154696e-06</v>
+        <v>4.9973621685239777e-08</v>
       </c>
     </row>
     <row r="211">
@@ -3689,7 +3689,7 @@
         <v>785624</v>
       </c>
       <c r="E211" s="1">
-        <v>1.9163073261552199e-07</v>
+        <v>6.9771601829415886e-09</v>
       </c>
     </row>
     <row r="212">
@@ -3706,7 +3706,7 @@
         <v>785624</v>
       </c>
       <c r="E212" s="1">
-        <v>1.7627039028411673e-07</v>
+        <v>6.4178991010521713e-09</v>
       </c>
     </row>
     <row r="213">
@@ -3723,7 +3723,7 @@
         <v>785624</v>
       </c>
       <c r="E213" s="1">
-        <v>2.0197680328237766e-07</v>
+        <v>7.3538544143048057e-09</v>
       </c>
     </row>
     <row r="214">
@@ -3740,7 +3740,7 @@
         <v>785624</v>
       </c>
       <c r="E214" s="1">
-        <v>9.2342571633707848e-07</v>
+        <v>3.3621375905568129e-08</v>
       </c>
     </row>
     <row r="215">
@@ -3757,7 +3757,7 @@
         <v>785624</v>
       </c>
       <c r="E215" s="1">
-        <v>1.6691428754711524e-06</v>
+        <v>6.0772492815885926e-08</v>
       </c>
     </row>
     <row r="216">
@@ -3774,7 +3774,7 @@
         <v>785624</v>
       </c>
       <c r="E216" s="1">
-        <v>1.4220426010069787e-06</v>
+        <v>5.1775717935242938e-08</v>
       </c>
     </row>
     <row r="217">
@@ -3791,7 +3791,7 @@
         <v>785624</v>
       </c>
       <c r="E217" s="1">
-        <v>5.7142602827298106e-07</v>
+        <v>2.0805277500812736e-08</v>
       </c>
     </row>
     <row r="218">
@@ -3808,7 +3808,7 @@
         <v>785624</v>
       </c>
       <c r="E218" s="1">
-        <v>3.4442444984961185e-07</v>
+        <v>1.2540287919193815e-08</v>
       </c>
     </row>
     <row r="219">
@@ -3825,7 +3825,7 @@
         <v>785624</v>
       </c>
       <c r="E219" s="1">
-        <v>2.0958808022442099e-07</v>
+        <v>7.6309758512138615e-09</v>
       </c>
     </row>
     <row r="220">
@@ -3842,7 +3842,7 @@
         <v>785624</v>
       </c>
       <c r="E220" s="1">
-        <v>2.2085718853759317e-07</v>
+        <v>8.0412778658001116e-09</v>
       </c>
     </row>
     <row r="221">
@@ -3859,7 +3859,7 @@
         <v>785624</v>
       </c>
       <c r="E221" s="1">
-        <v>3.4062637155329867e-07</v>
+        <v>1.2402002091960185e-08</v>
       </c>
     </row>
     <row r="222">
@@ -3876,7 +3876,7 @@
         <v>785624</v>
       </c>
       <c r="E222" s="1">
-        <v>3.0778610948800633e-07</v>
+        <v>1.1206307881650446e-08</v>
       </c>
     </row>
     <row r="223">
@@ -3893,7 +3893,7 @@
         <v>785624</v>
       </c>
       <c r="E223" s="1">
-        <v>3.2350840228900779e-07</v>
+        <v>1.1778746866752954e-08</v>
       </c>
     </row>
     <row r="224">
@@ -3910,7 +3910,7 @@
         <v>785624</v>
       </c>
       <c r="E224" s="1">
-        <v>2.0372112885524984e-07</v>
+        <v>7.417364056294673e-09</v>
       </c>
     </row>
     <row r="225">
@@ -3927,7 +3927,7 @@
         <v>785624</v>
       </c>
       <c r="E225" s="1">
-        <v>8.2248597266243451e-08</v>
+        <v>2.9946218838006189e-09</v>
       </c>
     </row>
     <row r="226">
@@ -3944,7 +3944,7 @@
         <v>785624</v>
       </c>
       <c r="E226" s="1">
-        <v>4.2072954897776071e-08</v>
+        <v>1.5318510904194227e-09</v>
       </c>
     </row>
     <row r="227">
@@ -3961,7 +3961,7 @@
         <v>785624</v>
       </c>
       <c r="E227" s="1">
-        <v>1.0736160405144801e-08</v>
+        <v>3.9089714798379305e-10</v>
       </c>
     </row>
     <row r="228">
@@ -3978,7 +3978,7 @@
         <v>785624</v>
       </c>
       <c r="E228" s="1">
-        <v>1.761674486844278e-11</v>
+        <v>6.4141508944459691e-13</v>
       </c>
     </row>
     <row r="229">
@@ -3995,7 +3995,7 @@
         <v>785624</v>
       </c>
       <c r="E229" s="1">
-        <v>1.4403329917644925e-10</v>
+        <v>5.2441657787116736e-12</v>
       </c>
     </row>
     <row r="230">
@@ -4012,7 +4012,7 @@
         <v>785624</v>
       </c>
       <c r="E230" s="1">
-        <v>5.173320971607609e-08</v>
+        <v>1.8835750736911905e-09</v>
       </c>
     </row>
     <row r="231">
@@ -4029,7 +4029,7 @@
         <v>785624</v>
       </c>
       <c r="E231" s="1">
-        <v>8.3288542729320625e-11</v>
+        <v>3.0324859377067748e-12</v>
       </c>
     </row>
     <row r="232">
@@ -4046,7 +4046,7 @@
         <v>785624</v>
       </c>
       <c r="E232" s="1">
-        <v>8.2260212530549381e-11</v>
+        <v>2.9950449672438983e-12</v>
       </c>
     </row>
     <row r="233">
@@ -4063,7 +4063,7 @@
         <v>785624</v>
       </c>
       <c r="E233" s="1">
-        <v>2.4018334543463027e-10</v>
+        <v>8.744930994619704e-12</v>
       </c>
     </row>
     <row r="234">
@@ -4080,7 +4080,7 @@
         <v>785624</v>
       </c>
       <c r="E234" s="1">
-        <v>6.1186938848933892e-10</v>
+        <v>2.2277797662173526e-11</v>
       </c>
     </row>
     <row r="235">
@@ -4097,7 +4097,7 @@
         <v>785624</v>
       </c>
       <c r="E235" s="1">
-        <v>9.1780416600073522e-10</v>
+        <v>3.3416699962707241e-11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>